<commit_message>
ajax kind of export
</commit_message>
<xml_diff>
--- a/public/file/test.xlsx
+++ b/public/file/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\res\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E7888-2CF9-4909-AC19-8683A2554D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78D4BC-59F6-48BE-A495-5CEEAE745BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12564" yWindow="744" windowWidth="10476" windowHeight="11616" xr2:uid="{AEF6103B-95B2-4995-96D4-4F4438B7AAB1}"/>
+    <workbookView xWindow="9072" yWindow="744" windowWidth="10476" windowHeight="11616" xr2:uid="{AEF6103B-95B2-4995-96D4-4F4438B7AAB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>qty</t>
   </si>
@@ -42,10 +42,13 @@
     <t>price</t>
   </si>
   <si>
-    <t>id_import</t>
-  </si>
-  <si>
-    <t>id_good</t>
+    <t>IP00034</t>
+  </si>
+  <si>
+    <t>code_import</t>
+  </si>
+  <si>
+    <t>id_material_detail</t>
   </si>
 </sst>
 </file>
@@ -400,20 +403,21 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -426,8 +430,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>8</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2">
         <v>52</v>
@@ -443,8 +447,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>8</v>
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
         <v>51</v>

</xml_diff>